<commit_message>
ajuste de funções e verificação de performance
</commit_message>
<xml_diff>
--- a/PREVENTIVA.xlsx
+++ b/PREVENTIVA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB32F5D-9707-4D20-98B1-5910FC098860}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07376084-F891-4268-9B99-D6062EBFB7EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="8">
   <si>
     <t>GOIANIA</t>
   </si>
@@ -33,22 +33,22 @@
     <t>APARECIDA DE GOIANIA</t>
   </si>
   <si>
-    <t>ANAPOLIS</t>
-  </si>
-  <si>
     <t>TRINDADE</t>
-  </si>
-  <si>
-    <t>APARECIDA DE GOI NIA</t>
   </si>
   <si>
     <t>SENADOR CANEDO</t>
   </si>
   <si>
+    <t>ANAPOLIS</t>
+  </si>
+  <si>
+    <t>BEZERRA (FORMOSA)</t>
+  </si>
+  <si>
     <t xml:space="preserve">REGIÃO </t>
   </si>
   <si>
-    <t xml:space="preserve">PEDIDO </t>
+    <t>PEDIDO</t>
   </si>
 </sst>
 </file>
@@ -366,17 +366,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B152"/>
+  <dimension ref="A1:B162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -391,7 +387,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1096995272</v>
+        <v>1097980801</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -399,55 +395,55 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1096883016</v>
+        <v>1097967399</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>1097003725</v>
+        <v>1097996073</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>1096881124</v>
+        <v>1097959620</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>1096968283</v>
+        <v>1097832759</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>1096880611</v>
+        <v>1097868057</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>1096931922</v>
+        <v>1097788908</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9">
-        <v>1097029558</v>
+        <v>1097857178</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -455,47 +451,47 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>1096286287</v>
+        <v>1097775747</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>1096292820</v>
+        <v>1097841593</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>1096270298</v>
+        <v>1097776089</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13">
-        <v>1096922930</v>
+        <v>1097981745</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>1096992072</v>
+        <v>1097973351</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>1096998859</v>
+        <v>1098007599</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -503,7 +499,7 @@
         <v>0</v>
       </c>
       <c r="B16">
-        <v>1096907555</v>
+        <v>1097981631</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -511,7 +507,7 @@
         <v>1</v>
       </c>
       <c r="B17">
-        <v>1096928178</v>
+        <v>1097956592</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -519,7 +515,7 @@
         <v>0</v>
       </c>
       <c r="B18">
-        <v>1096926912</v>
+        <v>1097984128</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -527,15 +523,15 @@
         <v>0</v>
       </c>
       <c r="B19">
-        <v>1096933271</v>
+        <v>1097742511</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>1096899634</v>
+        <v>1097956675</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -543,31 +539,31 @@
         <v>0</v>
       </c>
       <c r="B21">
-        <v>1096944897</v>
+        <v>1098054576</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B22">
-        <v>1096933844</v>
+        <v>1098008580</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B23">
-        <v>1096885717</v>
+        <v>1097978243</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B24">
-        <v>1096967890</v>
+        <v>1097953817</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -575,15 +571,15 @@
         <v>0</v>
       </c>
       <c r="B25">
-        <v>1096268518</v>
+        <v>1097938228</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>1096291521</v>
+        <v>1097998709</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -591,15 +587,15 @@
         <v>0</v>
       </c>
       <c r="B27">
-        <v>1096264195</v>
+        <v>1098006887</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B28">
-        <v>1096269293</v>
+        <v>1097959343</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -607,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="B29">
-        <v>1096885355</v>
+        <v>1097946586</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -615,39 +611,39 @@
         <v>0</v>
       </c>
       <c r="B30">
-        <v>1096946553</v>
+        <v>1097942049</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B31">
-        <v>1096963226</v>
+        <v>1097957169</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B32">
-        <v>1096894589</v>
+        <v>1097992587</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B33">
-        <v>1097032214</v>
+        <v>1098010820</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B34">
-        <v>1096901075</v>
+        <v>1097950125</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -655,7 +651,7 @@
         <v>0</v>
       </c>
       <c r="B35">
-        <v>1096934676</v>
+        <v>1097977245</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -663,15 +659,15 @@
         <v>0</v>
       </c>
       <c r="B36">
-        <v>1096947440</v>
+        <v>1097999408</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B37">
-        <v>1096960507</v>
+        <v>1097925411</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -679,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="B38">
-        <v>1096913706</v>
+        <v>1097915407</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -687,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="B39">
-        <v>1097039203</v>
+        <v>1097977342</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -695,7 +691,7 @@
         <v>0</v>
       </c>
       <c r="B40">
-        <v>1096937838</v>
+        <v>1097826932</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -703,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="B41">
-        <v>1096880791</v>
+        <v>1097857350</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -711,39 +707,39 @@
         <v>0</v>
       </c>
       <c r="B42">
-        <v>1096888535</v>
+        <v>1097828686</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B43">
-        <v>1096881771</v>
+        <v>1097855024</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B44">
-        <v>1097011649</v>
+        <v>1097780795</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B45">
-        <v>1096944121</v>
+        <v>1097850422</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B46">
-        <v>1096886870</v>
+        <v>1097778254</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -751,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="B47">
-        <v>1096273958</v>
+        <v>1097855826</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -759,23 +755,23 @@
         <v>0</v>
       </c>
       <c r="B48">
-        <v>1096308153</v>
+        <v>1097855853</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B49">
-        <v>1096276886</v>
+        <v>1097857271</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B50">
-        <v>1096279162</v>
+        <v>1097825975</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -783,23 +779,23 @@
         <v>0</v>
       </c>
       <c r="B51">
-        <v>1096295838</v>
+        <v>1097846203</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B52">
-        <v>1096273894</v>
+        <v>1097855063</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B53">
-        <v>1096295248</v>
+        <v>1095273443</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -807,7 +803,7 @@
         <v>0</v>
       </c>
       <c r="B54">
-        <v>1097029115</v>
+        <v>1098013282</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -815,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="B55">
-        <v>1096921754</v>
+        <v>1097970708</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -823,87 +819,87 @@
         <v>0</v>
       </c>
       <c r="B56">
-        <v>1097029156</v>
+        <v>1097904264</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B57">
-        <v>1096970085</v>
+        <v>1097983950</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B58">
-        <v>1097029157</v>
+        <v>1097965936</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B59">
-        <v>1096919586</v>
+        <v>1097871770</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B60">
-        <v>1097017186</v>
+        <v>1097835866</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B61">
-        <v>1097034006</v>
+        <v>1097820028</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B62">
-        <v>1097007661</v>
+        <v>1097862130</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B63">
-        <v>1096931660</v>
+        <v>1097798273</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B64">
-        <v>1097004502</v>
+        <v>1097859086</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B65">
-        <v>1097015583</v>
+        <v>1097815409</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B66">
-        <v>1096972776</v>
+        <v>1097760910</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -911,15 +907,15 @@
         <v>1</v>
       </c>
       <c r="B67">
-        <v>1096280722</v>
+        <v>1097993400</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B68">
-        <v>1097035972</v>
+        <v>1097967498</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -927,23 +923,23 @@
         <v>0</v>
       </c>
       <c r="B69">
-        <v>1096907328</v>
+        <v>1097905852</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B70">
-        <v>1096984100</v>
+        <v>1097828426</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B71">
-        <v>1096925232</v>
+        <v>1097861402</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -951,79 +947,79 @@
         <v>0</v>
       </c>
       <c r="B72">
-        <v>1097003565</v>
+        <v>1097837618</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B73">
-        <v>1096973412</v>
+        <v>1097834293</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B74">
-        <v>1096927814</v>
+        <v>1097950126</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B75">
-        <v>1096893984</v>
+        <v>1098008579</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B76">
-        <v>1096933412</v>
+        <v>1098008994</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B77">
-        <v>1096912511</v>
+        <v>1098011281</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B78">
-        <v>1097002048</v>
+        <v>1097901428</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B79">
-        <v>1096927718</v>
+        <v>1097978638</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B80">
-        <v>1096999838</v>
+        <v>1098007835</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B81">
-        <v>1097003566</v>
+        <v>1097822654</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1031,23 +1027,23 @@
         <v>0</v>
       </c>
       <c r="B82">
-        <v>1096966112</v>
+        <v>1097781191</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B83">
-        <v>1096909031</v>
+        <v>1097857938</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B84">
-        <v>1097024315</v>
+        <v>1097820802</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1055,39 +1051,39 @@
         <v>2</v>
       </c>
       <c r="B85">
-        <v>1097007118</v>
+        <v>1097824687</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B86">
-        <v>1097029107</v>
+        <v>1097806568</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B87">
-        <v>1097029108</v>
+        <v>1097870603</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B88">
-        <v>1096956652</v>
+        <v>1097841831</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B89">
-        <v>1097004698</v>
+        <v>1097961194</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1095,63 +1091,63 @@
         <v>0</v>
       </c>
       <c r="B90">
-        <v>1097009969</v>
+        <v>1097933192</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B91">
-        <v>1096927815</v>
+        <v>1097959767</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B92">
-        <v>1097006373</v>
+        <v>1097814852</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B93">
-        <v>1096900100</v>
+        <v>1097821982</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B94">
-        <v>1096940541</v>
+        <v>1097576340</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B95">
-        <v>1097012769</v>
+        <v>1097997693</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B96">
-        <v>1097002705</v>
+        <v>1097962119</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B97">
-        <v>1097003223</v>
+        <v>1097962902</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1159,31 +1155,31 @@
         <v>0</v>
       </c>
       <c r="B98">
-        <v>1096971713</v>
+        <v>1097896095</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B99">
-        <v>1096262259</v>
+        <v>1097883606</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B100">
-        <v>1096264069</v>
+        <v>1097857168</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B101">
-        <v>1096265400</v>
+        <v>1097874124</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -1191,55 +1187,55 @@
         <v>0</v>
       </c>
       <c r="B102">
-        <v>1096260860</v>
+        <v>1097819327</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B103">
-        <v>1096260861</v>
+        <v>1097873536</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B104">
-        <v>1096272063</v>
+        <v>1098047057</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B105">
-        <v>1096291124</v>
+        <v>1097815685</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B106">
-        <v>1096958662</v>
+        <v>1097819973</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B107">
-        <v>1096956121</v>
+        <v>1097780419</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B108">
-        <v>1096942270</v>
+        <v>1097824721</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -1247,23 +1243,23 @@
         <v>0</v>
       </c>
       <c r="B109">
-        <v>1097000966</v>
+        <v>1097787985</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B110">
-        <v>1096999741</v>
+        <v>1097810923</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B111">
-        <v>1096286321</v>
+        <v>1097799238</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -1271,95 +1267,95 @@
         <v>0</v>
       </c>
       <c r="B112">
-        <v>1096296389</v>
+        <v>1097823925</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B113">
-        <v>1096941730</v>
+        <v>1097915844</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B114">
-        <v>1096269922</v>
+        <v>1097996775</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B115">
-        <v>1096904229</v>
+        <v>1097806439</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B116">
-        <v>1096881115</v>
+        <v>1097833361</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B117">
-        <v>1096989462</v>
+        <v>1097869706</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B118">
-        <v>1096305655</v>
+        <v>1097821347</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B119">
-        <v>1096975245</v>
+        <v>1097844426</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B120">
-        <v>1096906332</v>
+        <v>1097563988</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B121">
-        <v>1097013329</v>
+        <v>1097941668</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B122">
-        <v>1096880438</v>
+        <v>1097901825</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B123">
-        <v>1096273439</v>
+        <v>1097920300</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -1367,15 +1363,15 @@
         <v>0</v>
       </c>
       <c r="B124">
-        <v>1096885828</v>
+        <v>1097875236</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B125">
-        <v>1096881511</v>
+        <v>1097777837</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -1383,55 +1379,55 @@
         <v>0</v>
       </c>
       <c r="B126">
-        <v>1096972510</v>
+        <v>1097779905</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B127">
-        <v>1096890654</v>
+        <v>1097782846</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B128">
-        <v>1096314707</v>
+        <v>1097955208</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B129">
-        <v>1096972456</v>
+        <v>1097907580</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B130">
-        <v>1096297199</v>
+        <v>1097986800</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B131">
-        <v>1096285328</v>
+        <v>1097965808</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B132">
-        <v>1096273089</v>
+        <v>1097877206</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -1439,7 +1435,7 @@
         <v>0</v>
       </c>
       <c r="B133">
-        <v>1096279169</v>
+        <v>1098009705</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -1447,15 +1443,15 @@
         <v>0</v>
       </c>
       <c r="B134">
-        <v>1096285383</v>
+        <v>1097915892</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B135">
-        <v>1096297386</v>
+        <v>1097973737</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -1463,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="B136">
-        <v>1096979327</v>
+        <v>1097982705</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -1471,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="B137">
-        <v>1096894599</v>
+        <v>1097947099</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -1479,15 +1475,15 @@
         <v>0</v>
       </c>
       <c r="B138">
-        <v>1096268494</v>
+        <v>1097870138</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B139">
-        <v>1096984691</v>
+        <v>1097805067</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -1495,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="B140">
-        <v>1096889748</v>
+        <v>1097781623</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -1503,31 +1499,31 @@
         <v>0</v>
       </c>
       <c r="B141">
-        <v>1096889265</v>
+        <v>1097784109</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B142">
-        <v>1097068625</v>
+        <v>1097842909</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B143">
-        <v>1097000333</v>
+        <v>1097860925</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B144">
-        <v>1097000955</v>
+        <v>1097851419</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -1535,15 +1531,15 @@
         <v>0</v>
       </c>
       <c r="B145">
-        <v>1096268383</v>
+        <v>1097813799</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B146">
-        <v>1096875873</v>
+        <v>1097803338</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -1551,23 +1547,23 @@
         <v>0</v>
       </c>
       <c r="B147">
-        <v>1096985725</v>
+        <v>1097955358</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B148">
-        <v>1097020925</v>
+        <v>1098016491</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B149">
-        <v>1096925121</v>
+        <v>1097977553</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -1575,23 +1571,103 @@
         <v>0</v>
       </c>
       <c r="B150">
-        <v>1096884846</v>
+        <v>1097902231</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B151">
-        <v>1097006862</v>
+        <v>1098052160</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B152">
-        <v>1096293067</v>
+        <v>1097862815</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>4</v>
+      </c>
+      <c r="B153">
+        <v>1097872466</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>0</v>
+      </c>
+      <c r="B154">
+        <v>1097813811</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>0</v>
+      </c>
+      <c r="B155">
+        <v>1097869174</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>0</v>
+      </c>
+      <c r="B156">
+        <v>1097797883</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>0</v>
+      </c>
+      <c r="B157">
+        <v>1097798172</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>0</v>
+      </c>
+      <c r="B158">
+        <v>1097826199</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>1</v>
+      </c>
+      <c r="B159">
+        <v>1097777061</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>1</v>
+      </c>
+      <c r="B160">
+        <v>1097720427</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>1</v>
+      </c>
+      <c r="B161">
+        <v>1097722099</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>1</v>
+      </c>
+      <c r="B162">
+        <v>1097559178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>